<commit_message>
Multimedia and Spreadsheet Data
</commit_message>
<xml_diff>
--- a/data_model_files/daschland (daschland)/resources.xlsx
+++ b/data_model_files/daschland (daschland)/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data_model_files/daschland (daschland)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data_model_files/daschland (daschland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B1E9BC-EEF1-5A4A-9ED5-89852563C1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A421C2-B734-0B4F-BD64-597A3E138028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="34220" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1546,10 +1546,10 @@
     <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="12" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="25.1640625" customWidth="1"/>
     <col min="13" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -2905,7 +2905,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+    <sheetView zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>

</xml_diff>